<commit_message>
buck bom list added
</commit_message>
<xml_diff>
--- a/Documenten/BOM PCB.xlsx
+++ b/Documenten/BOM PCB.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nielv\Documents\GitHub\CoolTeam\Documenten\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BasileBerckmoes\Documents\GitHub\CoolTeam\Documenten\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{82B6830D-26C5-41A9-9BF8-8DF67606203A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0750DFDB-A648-40B6-86C5-E7B963341789}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C4ACCA8C-4F35-4F2B-BD63-36B6377B3263}"/>
+    <workbookView xWindow="-150" yWindow="690" windowWidth="14055" windowHeight="11235" xr2:uid="{C4ACCA8C-4F35-4F2B-BD63-36B6377B3263}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="58">
   <si>
     <t>U1</t>
   </si>
@@ -81,9 +80,6 @@
     <t>ESP32-WROOM-32E 16MB</t>
   </si>
   <si>
-    <t>D1</t>
-  </si>
-  <si>
     <t>BAT760-7</t>
   </si>
   <si>
@@ -99,50 +95,125 @@
     <t xml:space="preserve">SMA CONNECTOR </t>
   </si>
   <si>
-    <t>https://www.mouser.be/ProductDetail/LPRS/SMA-CONNECTOR?qs=j%252B1pi9TdxUYkOiITvzJM8A%3D%3D</t>
-  </si>
-  <si>
     <t>C7</t>
   </si>
   <si>
     <t>C6</t>
   </si>
   <si>
-    <t>https://www.mouser.be/ProductDetail/Microchip-Technology/RN2483A-I-RM105?qs=sGAEpiMZZMu3sxpa5v1qrrZAnp88aoEUcCMjG6HT%2FSI%3D</t>
-  </si>
-  <si>
     <t>RN2483 module</t>
   </si>
   <si>
-    <t>https://www.mouser.be/ProductDetail/Texas-Instruments/TPS22860DBVR?qs=%2Fha2pyFadugxAdFBsj4zSHcoO0BzEMtLRhA2IvKn%252BB5VwA7fNnvmmg%3D%3D</t>
-  </si>
-  <si>
     <t xml:space="preserve">TPS22860DBVR </t>
   </si>
   <si>
-    <t>https://www.mouser.be/ProductDetail/KEMET/C0805C104K9RACAUTO?qs=ds50AKTGxA84SWre%252BvImOA%3D%3D</t>
-  </si>
-  <si>
     <t>C0805</t>
   </si>
   <si>
     <t>Condensator 100nF</t>
   </si>
   <si>
-    <t>https://www.mouser.be/ProductDetail/KEMET/C0805X105K8RAC7210?qs=ds50AKTGxA8Ac4j4qbsB5A%3D%3D</t>
-  </si>
-  <si>
     <t>Condensator 1µF</t>
   </si>
   <si>
     <t xml:space="preserve">sot-23 </t>
+  </si>
+  <si>
+    <t>D4</t>
+  </si>
+  <si>
+    <t>D1-D3</t>
+  </si>
+  <si>
+    <t>TPS563207DRLR</t>
+  </si>
+  <si>
+    <t>Locatie op schema</t>
+  </si>
+  <si>
+    <t>3: power</t>
+  </si>
+  <si>
+    <t>2: usb interface</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mouser </t>
+  </si>
+  <si>
+    <t>SOT563</t>
+  </si>
+  <si>
+    <t>cff</t>
+  </si>
+  <si>
+    <t>Rfbt</t>
+  </si>
+  <si>
+    <t>30.9 kOhms  1 %</t>
+  </si>
+  <si>
+    <t>10 kOhms 1%</t>
+  </si>
+  <si>
+    <t>Rfbb</t>
+  </si>
+  <si>
+    <t>r0603</t>
+  </si>
+  <si>
+    <t>Cin</t>
+  </si>
+  <si>
+    <t>c0603</t>
+  </si>
+  <si>
+    <t>cap, 39 pF, high q, 50 VDC</t>
+  </si>
+  <si>
+    <t>cap, 10 uF 20%, 25VDC</t>
+  </si>
+  <si>
+    <t>Cboot</t>
+  </si>
+  <si>
+    <t>cap, 0.1uF -20%,+80%, 16VDC</t>
+  </si>
+  <si>
+    <t>c0805</t>
+  </si>
+  <si>
+    <t>Cinx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cap 0.1uF 10%, 50VDC </t>
+  </si>
+  <si>
+    <t>U??</t>
+  </si>
+  <si>
+    <t>Cout</t>
+  </si>
+  <si>
+    <t>cap, 22uF 20%, 10VDC</t>
+  </si>
+  <si>
+    <t>c0806</t>
+  </si>
+  <si>
+    <t>L1</t>
+  </si>
+  <si>
+    <t>3,3 uH smoorspoel</t>
+  </si>
+  <si>
+    <t>smd 1307</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -163,6 +234,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -186,9 +263,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -504,23 +582,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C03AAE17-C990-4655-B41D-47FC550703C5}">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19:G20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.109375" customWidth="1"/>
-    <col min="2" max="2" width="27.33203125" customWidth="1"/>
-    <col min="3" max="3" width="14.44140625" customWidth="1"/>
+    <col min="1" max="1" width="14.140625" customWidth="1"/>
+    <col min="2" max="2" width="27.28515625" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" customWidth="1"/>
     <col min="4" max="4" width="14" customWidth="1"/>
-    <col min="5" max="5" width="11.88671875" customWidth="1"/>
-    <col min="6" max="6" width="12.5546875" customWidth="1"/>
+    <col min="5" max="5" width="5.85546875" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" customWidth="1"/>
+    <col min="7" max="7" width="21.7109375" customWidth="1"/>
+    <col min="8" max="8" width="17.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -539,8 +619,11 @@
       <c r="F1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -557,7 +640,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -574,7 +657,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -591,12 +674,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" t="s">
         <v>15</v>
-      </c>
-      <c r="B5" t="s">
-        <v>16</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -608,27 +691,36 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>29</v>
+      </c>
       <c r="B6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C6">
+        <v>3</v>
+      </c>
+      <c r="D6" t="s">
         <v>3</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="B7" t="s">
         <v>19</v>
       </c>
-      <c r="B7" t="s">
-        <v>20</v>
-      </c>
       <c r="C7">
         <v>1</v>
       </c>
@@ -636,15 +728,15 @@
         <v>3</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>0</v>
       </c>
       <c r="B8" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -653,61 +745,268 @@
         <v>3</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>5</v>
       </c>
       <c r="B9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9">
+        <v>3</v>
+      </c>
+      <c r="D9" t="s">
+        <v>3</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" t="s">
         <v>27</v>
       </c>
-      <c r="C9">
-        <v>3</v>
-      </c>
-      <c r="D9" t="s">
-        <v>3</v>
-      </c>
-      <c r="E9" s="1" t="s">
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" t="s">
+        <v>3</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" t="s">
         <v>26</v>
       </c>
-      <c r="F9" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>23</v>
-      </c>
-      <c r="B10" t="s">
+      <c r="D11" t="s">
+        <v>3</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>51</v>
+      </c>
+      <c r="B12" t="s">
         <v>30</v>
       </c>
-      <c r="D10" t="s">
-        <v>3</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F10" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>22</v>
-      </c>
-      <c r="B11" t="s">
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12" t="s">
+        <v>34</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F12" t="s">
+        <v>35</v>
+      </c>
+      <c r="G12" t="s">
         <v>32</v>
       </c>
-      <c r="D11" t="s">
-        <v>3</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F11" t="s">
-        <v>29</v>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" t="s">
+        <v>44</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13" t="s">
+        <v>3</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F13" t="s">
+        <v>43</v>
+      </c>
+      <c r="G13" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>37</v>
+      </c>
+      <c r="B14" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14" t="s">
+        <v>3</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F14" t="s">
+        <v>41</v>
+      </c>
+      <c r="G14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B15" t="s">
+        <v>39</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15" t="s">
+        <v>3</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F15" t="s">
+        <v>41</v>
+      </c>
+      <c r="G15" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>42</v>
+      </c>
+      <c r="B16" t="s">
+        <v>45</v>
+      </c>
+      <c r="C16">
+        <v>2</v>
+      </c>
+      <c r="D16" t="s">
+        <v>3</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F16" t="s">
+        <v>48</v>
+      </c>
+      <c r="G16" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>46</v>
+      </c>
+      <c r="B17" t="s">
+        <v>47</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17" t="s">
+        <v>3</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F17" t="s">
+        <v>43</v>
+      </c>
+      <c r="G17" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>49</v>
+      </c>
+      <c r="B18" t="s">
+        <v>50</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F18" t="s">
+        <v>48</v>
+      </c>
+      <c r="G18" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>52</v>
+      </c>
+      <c r="B19" t="s">
+        <v>53</v>
+      </c>
+      <c r="C19">
+        <v>2</v>
+      </c>
+      <c r="D19" t="s">
+        <v>3</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F19" t="s">
+        <v>54</v>
+      </c>
+      <c r="G19" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>55</v>
+      </c>
+      <c r="B20" t="s">
+        <v>56</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20" t="s">
+        <v>3</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F20" t="s">
+        <v>57</v>
+      </c>
+      <c r="G20" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -723,7 +1022,17 @@
     <hyperlink ref="E9" r:id="rId8" xr:uid="{00215C6C-F998-4D8B-9F6B-10A7C1F6E707}"/>
     <hyperlink ref="E10" r:id="rId9" xr:uid="{A86CAC7B-104C-4AB9-95C8-FC36A3F7664E}"/>
     <hyperlink ref="E11" r:id="rId10" xr:uid="{A34CC104-BAA9-45DC-94CF-43986FFA8FA8}"/>
+    <hyperlink ref="E12" r:id="rId11" xr:uid="{111EA3D2-92D2-450F-8CBB-5D974F638569}"/>
+    <hyperlink ref="E13" r:id="rId12" xr:uid="{6499BC8A-8DC9-45FA-BD0E-EB060369E9E4}"/>
+    <hyperlink ref="E14" r:id="rId13" xr:uid="{CB3B99D8-27D5-481A-B110-E6ED7A32BC0A}"/>
+    <hyperlink ref="E15" r:id="rId14" xr:uid="{5C7FA240-1D82-4990-BFA1-8D8EF2C066F4}"/>
+    <hyperlink ref="E16" r:id="rId15" xr:uid="{730D95A2-4AA0-447D-8C34-2C11C16DB3E8}"/>
+    <hyperlink ref="E17" r:id="rId16" xr:uid="{DC0594E2-19B7-4E44-A894-95DC3F881CE8}"/>
+    <hyperlink ref="E18" r:id="rId17" xr:uid="{4CFBF430-7559-47A5-8B25-C2560DA004EB}"/>
+    <hyperlink ref="E19" r:id="rId18" xr:uid="{5047CDD3-8734-4EE4-BCD6-DB431A819AFB}"/>
+    <hyperlink ref="E20" r:id="rId19" xr:uid="{C0B0478A-E6CA-4D76-92C9-097B430F4063}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId20"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
buck added (shcema en bom)
</commit_message>
<xml_diff>
--- a/Documenten/BOM PCB.xlsx
+++ b/Documenten/BOM PCB.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BasileBerckmoes\Documents\GitHub\CoolTeam\Documenten\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0750DFDB-A648-40B6-86C5-E7B963341789}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5559995-A17A-4D3E-BBBB-F68D61515346}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-150" yWindow="690" windowWidth="14055" windowHeight="11235" xr2:uid="{C4ACCA8C-4F35-4F2B-BD63-36B6377B3263}"/>
+    <workbookView xWindow="12870" yWindow="1980" windowWidth="14850" windowHeight="11235" xr2:uid="{C4ACCA8C-4F35-4F2B-BD63-36B6377B3263}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="60">
   <si>
     <t>U1</t>
   </si>
@@ -197,9 +197,6 @@
     <t>cap, 22uF 20%, 10VDC</t>
   </si>
   <si>
-    <t>c0806</t>
-  </si>
-  <si>
     <t>L1</t>
   </si>
   <si>
@@ -207,6 +204,15 @@
   </si>
   <si>
     <t>smd 1307</t>
+  </si>
+  <si>
+    <t>NOG NIET ALLE CAPS EN WEERSTANDEN STAAN IN BOM!!!</t>
+  </si>
+  <si>
+    <t>IC2</t>
+  </si>
+  <si>
+    <t>IC1</t>
   </si>
 </sst>
 </file>
@@ -263,10 +269,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -582,10 +589,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C03AAE17-C990-4655-B41D-47FC550703C5}">
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19:G20"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -600,7 +607,7 @@
     <col min="8" max="8" width="17.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -623,9 +630,9 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>59</v>
       </c>
       <c r="B2" t="s">
         <v>14</v>
@@ -640,9 +647,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>58</v>
       </c>
       <c r="B3" t="s">
         <v>9</v>
@@ -657,7 +664,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -674,7 +681,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>28</v>
       </c>
@@ -691,7 +698,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>29</v>
       </c>
@@ -714,7 +721,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -731,7 +738,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>0</v>
       </c>
@@ -748,7 +755,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -768,7 +775,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>21</v>
       </c>
@@ -784,8 +791,11 @@
       <c r="F10" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H10" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -802,7 +812,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>51</v>
       </c>
@@ -825,7 +835,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>36</v>
       </c>
@@ -848,7 +858,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>37</v>
       </c>
@@ -871,7 +881,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>40</v>
       </c>
@@ -894,7 +904,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>42</v>
       </c>
@@ -980,7 +990,7 @@
         <v>12</v>
       </c>
       <c r="F19" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="G19" t="s">
         <v>32</v>
@@ -988,26 +998,29 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>54</v>
+      </c>
+      <c r="B20" t="s">
         <v>55</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20" t="s">
+        <v>3</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F20" t="s">
         <v>56</v>
-      </c>
-      <c r="C20">
-        <v>1</v>
-      </c>
-      <c r="D20" t="s">
-        <v>3</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F20" t="s">
-        <v>57</v>
       </c>
       <c r="G20" t="s">
         <v>32</v>
       </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E21" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
laatste componenten en pcb2 toegevoegd
</commit_message>
<xml_diff>
--- a/Documenten/BOM PCB.xlsx
+++ b/Documenten/BOM PCB.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BasileBerckmoes\Documents\GitHub\CoolTeam\Documenten\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ADDF952-03FA-4578-A961-8F95DE6DE41B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0026A7B3-BC69-488B-8192-36173FB3C9F4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16320" yWindow="1860" windowWidth="14850" windowHeight="11235" xr2:uid="{C4ACCA8C-4F35-4F2B-BD63-36B6377B3263}"/>
+    <workbookView xWindow="8430" yWindow="2220" windowWidth="14850" windowHeight="11235" xr2:uid="{C4ACCA8C-4F35-4F2B-BD63-36B6377B3263}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="35">
   <si>
     <t>U1</t>
   </si>
@@ -74,9 +74,6 @@
     <t xml:space="preserve">SMA CONNECTOR </t>
   </si>
   <si>
-    <t>C7</t>
-  </si>
-  <si>
     <t>RN2483 module</t>
   </si>
   <si>
@@ -89,9 +86,6 @@
     <t xml:space="preserve">sot-23 </t>
   </si>
   <si>
-    <t>Locatie op schema</t>
-  </si>
-  <si>
     <t>LDO 2-10V In, 3,3v out, 35uA sleep</t>
   </si>
   <si>
@@ -101,12 +95,6 @@
     <t>U3</t>
   </si>
   <si>
-    <t>1:ESP32</t>
-  </si>
-  <si>
-    <t>4:Power</t>
-  </si>
-  <si>
     <t>U4</t>
   </si>
   <si>
@@ -141,6 +129,15 @@
   </si>
   <si>
     <t>4k6 0805</t>
+  </si>
+  <si>
+    <t>5 pin molex connector</t>
+  </si>
+  <si>
+    <t>2 pin molex connector</t>
+  </si>
+  <si>
+    <t>C4,C5,C7</t>
   </si>
 </sst>
 </file>
@@ -510,10 +507,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C03AAE17-C990-4655-B41D-47FC550703C5}">
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -528,7 +525,7 @@
     <col min="8" max="8" width="17.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -547,13 +544,10 @@
       <c r="F1" t="s">
         <v>7</v>
       </c>
-      <c r="G1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B2" t="s">
         <v>10</v>
@@ -567,11 +561,8 @@
       <c r="E2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -588,12 +579,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>0</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -605,12 +596,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C5">
         <v>3</v>
@@ -622,15 +613,15 @@
         <v>9</v>
       </c>
       <c r="F5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B6" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C6">
         <v>5</v>
@@ -642,15 +633,15 @@
         <v>9</v>
       </c>
       <c r="F6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>34</v>
       </c>
       <c r="B7" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C7">
         <v>6</v>
@@ -662,15 +653,15 @@
         <v>9</v>
       </c>
       <c r="F7" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B8" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -682,34 +673,34 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B9" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C9">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B10" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C10">
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B11" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -721,18 +712,15 @@
         <v>9</v>
       </c>
       <c r="F11" t="s">
-        <v>20</v>
-      </c>
-      <c r="G11" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B12" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C12">
         <v>2</v>
@@ -741,6 +729,34 @@
         <v>3</v>
       </c>
       <c r="E12" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13">
+        <v>2</v>
+      </c>
+      <c r="D13" t="s">
+        <v>3</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14" t="s">
+        <v>3</v>
+      </c>
+      <c r="E14" s="1" t="s">
         <v>9</v>
       </c>
     </row>
@@ -759,8 +775,10 @@
     <hyperlink ref="E11" r:id="rId7" xr:uid="{2DEF7EAC-6C67-5341-B973-214106A156C4}"/>
     <hyperlink ref="E12" r:id="rId8" xr:uid="{607CC1AF-A389-4D80-87CD-CE91C0E6B71E}"/>
     <hyperlink ref="E8" r:id="rId9" xr:uid="{AAF30544-E85A-4F12-BCE4-F8C712C81B9F}"/>
+    <hyperlink ref="E13" r:id="rId10" xr:uid="{AC83962E-4A0D-47D6-B951-0E42BB51283B}"/>
+    <hyperlink ref="E14" r:id="rId11" xr:uid="{03C25817-B479-4457-B806-9A0525E20E00}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId10"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId12"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
export pcb1 aangepast, BOM PCB aangepast
</commit_message>
<xml_diff>
--- a/Documenten/BOM PCB.xlsx
+++ b/Documenten/BOM PCB.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/manoelledeviron/Documents/KUL/2020-2021/IoT Nodes/Labo/CoolTeam/Documenten/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50116900-4D85-A44F-A851-1CE4F63898A1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0826ABE2-0026-574C-91E9-A3D7E0F1EB79}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15840" xr2:uid="{C4ACCA8C-4F35-4F2B-BD63-36B6377B3263}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{C4ACCA8C-4F35-4F2B-BD63-36B6377B3263}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="38">
   <si>
     <t>U1</t>
   </si>
@@ -50,9 +50,6 @@
     <t>Leverancier</t>
   </si>
   <si>
-    <t>U2</t>
-  </si>
-  <si>
     <t>Aantal</t>
   </si>
   <si>
@@ -119,9 +116,6 @@
     <t>10k 0805</t>
   </si>
   <si>
-    <t>R2, R3</t>
-  </si>
-  <si>
     <t>5 pin molex connector</t>
   </si>
   <si>
@@ -131,34 +125,28 @@
     <t>female pinheader 8</t>
   </si>
   <si>
-    <t>4k7 0805</t>
-  </si>
-  <si>
-    <t>R1, R6, R7</t>
-  </si>
-  <si>
-    <t>C1,C2,C6,C8,C9,C11,C12</t>
-  </si>
-  <si>
-    <t>C4,C5,C7,C10,C13</t>
-  </si>
-  <si>
     <t>U7</t>
   </si>
   <si>
-    <t>PA1010-D</t>
-  </si>
-  <si>
-    <t>L1</t>
-  </si>
-  <si>
-    <t>MFBM1V1005-501-R</t>
-  </si>
-  <si>
-    <t>L0402</t>
-  </si>
-  <si>
-    <t>te zien met cd technology</t>
+    <t>Adafruit Mini GPS</t>
+  </si>
+  <si>
+    <t>al gekocht</t>
+  </si>
+  <si>
+    <t>female pinheader 6</t>
+  </si>
+  <si>
+    <t>U2,U6,</t>
+  </si>
+  <si>
+    <t>R1,R2,R3</t>
+  </si>
+  <si>
+    <t>C4,C5,C7,C13</t>
+  </si>
+  <si>
+    <t>C1,C2,C6,C8,C9,C11</t>
   </si>
 </sst>
 </file>
@@ -528,10 +516,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C03AAE17-C990-4655-B41D-47FC550703C5}">
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -546,7 +534,7 @@
     <col min="8" max="8" width="17.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -554,24 +542,24 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D1" t="s">
         <v>4</v>
       </c>
       <c r="E1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -580,15 +568,15 @@
         <v>3</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
         <v>11</v>
-      </c>
-      <c r="B3" t="s">
-        <v>12</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -597,15 +585,15 @@
         <v>3</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>0</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -614,15 +602,15 @@
         <v>3</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>34</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C5">
         <v>3</v>
@@ -631,18 +619,18 @@
         <v>3</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C6">
         <v>7</v>
@@ -651,18 +639,18 @@
         <v>3</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C7">
         <v>5</v>
@@ -671,18 +659,18 @@
         <v>3</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F7" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" t="s">
         <v>25</v>
-      </c>
-      <c r="B8" t="s">
-        <v>26</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -691,66 +679,66 @@
         <v>3</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9">
+        <v>3</v>
+      </c>
+      <c r="D9" t="s">
+        <v>3</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10" t="s">
+        <v>3</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11">
+        <v>2</v>
+      </c>
+      <c r="D11" t="s">
+        <v>3</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
         <v>27</v>
-      </c>
-      <c r="C9">
-        <v>3</v>
-      </c>
-      <c r="D9" t="s">
-        <v>3</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>28</v>
-      </c>
-      <c r="B10" t="s">
-        <v>32</v>
-      </c>
-      <c r="C10">
-        <v>2</v>
-      </c>
-      <c r="D10" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11" t="s">
-        <v>17</v>
-      </c>
-      <c r="C11">
-        <v>1</v>
-      </c>
-      <c r="D11" t="s">
-        <v>3</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F11" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>22</v>
-      </c>
-      <c r="B12" t="s">
-        <v>21</v>
       </c>
       <c r="C12">
         <v>2</v>
@@ -759,90 +747,71 @@
         <v>3</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13" t="s">
+        <v>3</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
         <v>29</v>
       </c>
-      <c r="C13">
+      <c r="C14">
         <v>2</v>
       </c>
-      <c r="D13" t="s">
-        <v>3</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B14" t="s">
+      <c r="D14" t="s">
+        <v>3</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
         <v>30</v>
       </c>
-      <c r="C14">
-        <v>1</v>
-      </c>
-      <c r="D14" t="s">
-        <v>3</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
         <v>31</v>
       </c>
       <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15" t="s">
+        <v>3</v>
+      </c>
+      <c r="E15" s="1"/>
+      <c r="G15" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16">
         <v>2</v>
       </c>
-      <c r="D15" t="s">
-        <v>3</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>36</v>
-      </c>
-      <c r="B16" t="s">
-        <v>37</v>
-      </c>
-      <c r="C16">
-        <v>1</v>
-      </c>
       <c r="D16" t="s">
-        <v>41</v>
+        <v>3</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>38</v>
-      </c>
-      <c r="B17" t="s">
-        <v>39</v>
-      </c>
-      <c r="C17">
-        <v>1</v>
-      </c>
-      <c r="D17" t="s">
-        <v>3</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F17" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="E21" s="2"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E20" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -853,17 +822,16 @@
     <hyperlink ref="E5" r:id="rId4" xr:uid="{00215C6C-F998-4D8B-9F6B-10A7C1F6E707}"/>
     <hyperlink ref="E6" r:id="rId5" xr:uid="{A86CAC7B-104C-4AB9-95C8-FC36A3F7664E}"/>
     <hyperlink ref="E7" r:id="rId6" xr:uid="{A34CC104-BAA9-45DC-94CF-43986FFA8FA8}"/>
-    <hyperlink ref="E11" r:id="rId7" xr:uid="{2DEF7EAC-6C67-5341-B973-214106A156C4}"/>
-    <hyperlink ref="E12" r:id="rId8" xr:uid="{607CC1AF-A389-4D80-87CD-CE91C0E6B71E}"/>
+    <hyperlink ref="E10" r:id="rId7" xr:uid="{2DEF7EAC-6C67-5341-B973-214106A156C4}"/>
+    <hyperlink ref="E11" r:id="rId8" xr:uid="{607CC1AF-A389-4D80-87CD-CE91C0E6B71E}"/>
     <hyperlink ref="E8" r:id="rId9" xr:uid="{AAF30544-E85A-4F12-BCE4-F8C712C81B9F}"/>
-    <hyperlink ref="E13" r:id="rId10" xr:uid="{AC83962E-4A0D-47D6-B951-0E42BB51283B}"/>
-    <hyperlink ref="E14" r:id="rId11" xr:uid="{03C25817-B479-4457-B806-9A0525E20E00}"/>
-    <hyperlink ref="E15" r:id="rId12" xr:uid="{B3A1F735-A7F6-496F-8C06-9BCE3F069E56}"/>
+    <hyperlink ref="E12" r:id="rId10" xr:uid="{AC83962E-4A0D-47D6-B951-0E42BB51283B}"/>
+    <hyperlink ref="E13" r:id="rId11" xr:uid="{03C25817-B479-4457-B806-9A0525E20E00}"/>
+    <hyperlink ref="E14" r:id="rId12" xr:uid="{B3A1F735-A7F6-496F-8C06-9BCE3F069E56}"/>
     <hyperlink ref="E9" r:id="rId13" xr:uid="{47D3745D-E199-4093-A430-24E5A475A1E6}"/>
-    <hyperlink ref="E17" r:id="rId14" xr:uid="{1E251AFD-0D35-C248-A8E7-4CABDAE5F4F3}"/>
-    <hyperlink ref="E16" r:id="rId15" xr:uid="{43C854E1-6A11-EE4E-BBAC-993579D30E7F}"/>
+    <hyperlink ref="E16" r:id="rId14" xr:uid="{ED94B40A-32B1-044F-8A22-28C8BEAC0A8E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId16"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId15"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
main code Basile aangepast met GPS
</commit_message>
<xml_diff>
--- a/Documenten/BOM PCB.xlsx
+++ b/Documenten/BOM PCB.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nielv\Documents\GitHub\CoolTeam\Documenten\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/manoelledeviron/Documents/KUL/2020-2021/IoT Nodes/Labo/CoolTeam/Documenten/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B08D1812-2BFB-47BC-9D1A-444517976800}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2655389-E9C8-904E-818F-29E6AE82D2B6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C4ACCA8C-4F35-4F2B-BD63-36B6377B3263}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="23260" windowHeight="12580" xr2:uid="{C4ACCA8C-4F35-4F2B-BD63-36B6377B3263}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -471,7 +471,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -487,7 +487,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -786,25 +786,25 @@
   <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L23" sqref="L23"/>
+      <selection activeCell="B13" sqref="B12:B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.44140625" customWidth="1"/>
-    <col min="2" max="2" width="29.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.109375" customWidth="1"/>
-    <col min="6" max="6" width="16.5546875" customWidth="1"/>
+    <col min="1" max="1" width="17.5" customWidth="1"/>
+    <col min="2" max="2" width="29.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.1640625" customWidth="1"/>
+    <col min="6" max="6" width="16.5" customWidth="1"/>
     <col min="7" max="7" width="14" customWidth="1"/>
-    <col min="8" max="8" width="5.77734375" customWidth="1"/>
-    <col min="9" max="9" width="12.44140625" customWidth="1"/>
+    <col min="8" max="8" width="5.83203125" customWidth="1"/>
+    <col min="9" max="9" width="12.5" customWidth="1"/>
     <col min="10" max="10" width="21.6640625" customWidth="1"/>
-    <col min="11" max="11" width="17.44140625" customWidth="1"/>
+    <col min="11" max="11" width="17.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>1</v>
       </c>
@@ -839,7 +839,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
         <v>16</v>
       </c>
@@ -875,7 +875,7 @@
         <v>5.28</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
         <v>9</v>
       </c>
@@ -911,7 +911,7 @@
         <v>2.14</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
         <v>0</v>
       </c>
@@ -947,7 +947,7 @@
         <v>22.76</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="s">
         <v>30</v>
       </c>
@@ -985,7 +985,7 @@
         <v>6.5759999999999996</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="9" t="s">
         <v>33</v>
       </c>
@@ -1023,7 +1023,7 @@
         <v>2.73</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
         <v>32</v>
       </c>
@@ -1061,7 +1061,7 @@
         <v>6.18</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="9" t="s">
         <v>22</v>
       </c>
@@ -1097,7 +1097,7 @@
         <v>0.55200000000000005</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="9" t="s">
         <v>31</v>
       </c>
@@ -1135,7 +1135,7 @@
         <v>0.52</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="9" t="s">
         <v>17</v>
       </c>
@@ -1173,7 +1173,7 @@
         <v>2.133</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="9" t="s">
         <v>19</v>
       </c>
@@ -1209,7 +1209,7 @@
         <v>2.2000000000000002</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="9"/>
       <c r="B12" s="2" t="s">
         <v>24</v>
@@ -1243,7 +1243,7 @@
         <v>8.9600000000000009</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="9"/>
       <c r="B13" s="2" t="s">
         <v>25</v>
@@ -1277,7 +1277,7 @@
         <v>1.762</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="9"/>
       <c r="B14" s="2" t="s">
         <v>26</v>
@@ -1311,7 +1311,7 @@
         <v>2.012</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="9" t="s">
         <v>27</v>
       </c>
@@ -1347,7 +1347,7 @@
         <v>25.37</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="9"/>
       <c r="B16" s="2" t="s">
         <v>29</v>
@@ -1381,7 +1381,7 @@
         <v>2.4159999999999999</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="9" t="s">
         <v>37</v>
       </c>
@@ -1417,7 +1417,7 @@
         <v>9.4600000000000009</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
         <v>37</v>
       </c>
@@ -1453,7 +1453,7 @@
         <v>14.7</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="J19" s="16" t="s">
         <v>47</v>
       </c>
@@ -1462,13 +1462,13 @@
         <v>115.75100000000002</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B20" s="18" t="s">
         <v>45</v>
       </c>
       <c r="H20" s="1"/>
     </row>
-    <row r="21" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B21" s="19">
         <v>2</v>
       </c>

</xml_diff>